<commit_message>
Correcoes do sentidos no Diagrama das tasks
</commit_message>
<xml_diff>
--- a/Documentos/Tasks.xlsx
+++ b/Documentos/Tasks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\workspace\GoodsTracker\Documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="9285"/>
   </bookViews>
@@ -15,14 +20,18 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -50,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -62,6 +72,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -83,7 +96,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -133,25 +152,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6172200" y="800100"/>
+          <a:off x="6057900" y="800100"/>
           <a:ext cx="0" cy="4800600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -193,7 +218,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -256,7 +287,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -319,7 +356,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -382,75 +425,18 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1790701" y="4162424"/>
-          <a:ext cx="720000" cy="1080000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="3175"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Accelerometer</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>462826</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>98925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="962026" y="4162425"/>
           <a:ext cx="720000" cy="1080000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -495,6 +481,75 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>462826</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>98925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="962026" y="4162425"/>
+          <a:ext cx="720000" cy="1080000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="3175"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Accel</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>123826</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -508,7 +563,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -567,17 +628,23 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="762000" y="647700"/>
-          <a:ext cx="1038225" cy="495300"/>
+          <a:ext cx="1038225" cy="533400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -621,32 +688,40 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>213825</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>351451</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:colOff>485776</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Elbow Connector 13"/>
+        <xdr:cNvPr id="14" name="Elbow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="6" idx="1"/>
-          <a:endCxn id="130" idx="0"/>
+          <a:endCxn id="132" idx="6"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="4481025" y="1238249"/>
-          <a:ext cx="3929550" cy="1704975"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+          <a:off x="4009051" y="1238250"/>
+          <a:ext cx="4401525" cy="2280750"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -684,7 +759,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15"/>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -747,7 +828,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Rectangle 19"/>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -810,7 +897,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectangle 20"/>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -873,7 +966,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="Rectangle 21"/>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -936,7 +1035,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Elbow Connector 16"/>
+        <xdr:cNvPr id="17" name="Elbow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="127" idx="2"/>
           <a:endCxn id="8" idx="2"/>
@@ -987,7 +1092,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:endCxn id="21" idx="3"/>
         </xdr:cNvCxnSpPr>
@@ -1037,7 +1148,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="Rectangle 54"/>
+        <xdr:cNvPr id="55" name="Rectangle 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1100,7 +1217,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Straight Arrow Connector 65"/>
+        <xdr:cNvPr id="66" name="Straight Arrow Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:endCxn id="22" idx="3"/>
         </xdr:cNvCxnSpPr>
@@ -1150,7 +1273,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="71" name="Elbow Connector 70"/>
+        <xdr:cNvPr id="71" name="Elbow Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="11" idx="0"/>
           <a:endCxn id="55" idx="1"/>
@@ -1200,7 +1329,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Elbow Connector 72"/>
+        <xdr:cNvPr id="73" name="Elbow Connector 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000049000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="0"/>
           <a:endCxn id="55" idx="1"/>
@@ -1253,7 +1388,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Elbow Connector 73"/>
+        <xdr:cNvPr id="74" name="Elbow Connector 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="0"/>
           <a:endCxn id="55" idx="1"/>
@@ -1294,19 +1435,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>321901</xdr:colOff>
+      <xdr:colOff>321900</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>575775</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261449</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>98924</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="89" name="Elbow Connector 88"/>
+        <xdr:cNvPr id="89" name="Elbow Connector 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000059000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="2"/>
           <a:endCxn id="132" idx="4"/>
@@ -1314,8 +1461,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="2070526" y="3689175"/>
-          <a:ext cx="1633424" cy="1473074"/>
+          <a:off x="2218163" y="3541537"/>
+          <a:ext cx="1633424" cy="1768349"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1346,19 +1493,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>102825</xdr:colOff>
+      <xdr:colOff>102826</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>575774</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261450</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>98925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="91" name="Elbow Connector 90"/>
+        <xdr:cNvPr id="91" name="Elbow Connector 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="10" idx="2"/>
           <a:endCxn id="132" idx="4"/>
@@ -1366,8 +1519,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="1656187" y="3274838"/>
-          <a:ext cx="1633425" cy="2301749"/>
+          <a:off x="1803825" y="3127201"/>
+          <a:ext cx="1633425" cy="2597024"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1398,19 +1551,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>483825</xdr:colOff>
+      <xdr:colOff>483826</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>575774</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>261450</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>108449</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="93" name="Elbow Connector 92"/>
+        <xdr:cNvPr id="93" name="Elbow Connector 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="11" idx="2"/>
           <a:endCxn id="132" idx="4"/>
@@ -1418,8 +1577,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="1232325" y="2860500"/>
-          <a:ext cx="1642949" cy="3139949"/>
+          <a:off x="1379963" y="2712863"/>
+          <a:ext cx="1642949" cy="3435224"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1457,7 +1616,13 @@
     <xdr:ext cx="877741" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="121" name="TextBox 120"/>
+        <xdr:cNvPr id="121" name="TextBox 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000079000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1509,7 +1674,13 @@
     <xdr:ext cx="877741" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="122" name="TextBox 121"/>
+        <xdr:cNvPr id="122" name="TextBox 121">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1553,20 +1724,26 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="877741" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="123" name="TextBox 122"/>
+        <xdr:cNvPr id="123" name="TextBox 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2571750" y="5229225"/>
+          <a:off x="3086100" y="5229225"/>
           <a:ext cx="877741" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1613,7 +1790,13 @@
     <xdr:ext cx="964688" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="124" name="TextBox 123"/>
+        <xdr:cNvPr id="124" name="TextBox 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1665,7 +1848,13 @@
     <xdr:ext cx="964688" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="125" name="TextBox 124"/>
+        <xdr:cNvPr id="125" name="TextBox 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1717,7 +1906,13 @@
     <xdr:ext cx="964688" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="TextBox 128"/>
+        <xdr:cNvPr id="129" name="TextBox 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1774,7 +1969,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="47" name="Elbow Connector 46"/>
+        <xdr:cNvPr id="47" name="Elbow Connector 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="55" idx="3"/>
           <a:endCxn id="8" idx="1"/>
@@ -1816,22 +2017,28 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>427657</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="70" name="Rectangle 69"/>
+        <xdr:cNvPr id="70" name="Rectangle 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2657475" y="4591050"/>
+          <a:off x="2657475" y="4572000"/>
           <a:ext cx="818182" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1882,32 +2089,38 @@
       <xdr:rowOff>130424</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>18566</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Elbow Connector 74"/>
+        <xdr:cNvPr id="75" name="Elbow Connector 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="9" idx="3"/>
-          <a:endCxn id="70" idx="2"/>
+          <a:endCxn id="70" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2510701" y="4702424"/>
-          <a:ext cx="555865" cy="155326"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector4">
+          <a:ext cx="146774" cy="2926"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 13202"/>
-            <a:gd name="adj2" fmla="val 247174"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
-          <a:tailEnd type="arrow"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="none"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1931,23 +2144,29 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Double Bracket 49"/>
+        <xdr:cNvPr id="50" name="Double Bracket 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4029075" y="5257800"/>
+          <a:off x="4029075" y="6143625"/>
           <a:ext cx="809625" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="bracketPair">
@@ -1986,33 +2205,36 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>18567</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>371476</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>176214</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="Elbow Connector 75"/>
+        <xdr:cNvPr id="76" name="Elbow Connector 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00004C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="50" idx="1"/>
-          <a:endCxn id="70" idx="0"/>
+          <a:endCxn id="70" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3066567" y="4591051"/>
-          <a:ext cx="962509" cy="919163"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector4">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 28749"/>
-            <a:gd name="adj2" fmla="val 124870"/>
-          </a:avLst>
+          <a:off x="3066567" y="4838700"/>
+          <a:ext cx="962509" cy="1557338"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -2050,7 +2272,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="86" name="Double Bracket 85"/>
+        <xdr:cNvPr id="86" name="Double Bracket 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2105,7 +2333,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="87" name="Elbow Connector 86"/>
+        <xdr:cNvPr id="87" name="Elbow Connector 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000057000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="86" idx="1"/>
           <a:endCxn id="16" idx="2"/>
@@ -2155,7 +2389,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="94" name="Straight Arrow Connector 93"/>
+        <xdr:cNvPr id="94" name="Straight Arrow Connector 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="16" idx="0"/>
           <a:endCxn id="6" idx="2"/>
@@ -2170,8 +2410,8 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:headEnd type="arrow" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2206,7 +2446,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="96" name="Straight Arrow Connector 95"/>
+        <xdr:cNvPr id="96" name="Straight Arrow Connector 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="20" idx="2"/>
           <a:endCxn id="7" idx="0"/>
@@ -2257,7 +2503,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="Double Bracket 98"/>
+        <xdr:cNvPr id="99" name="Double Bracket 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2312,7 +2564,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="101" name="Elbow Connector 100"/>
+        <xdr:cNvPr id="101" name="Elbow Connector 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000065000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="99" idx="1"/>
           <a:endCxn id="20" idx="0"/>
@@ -2327,7 +2585,8 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:tailEnd type="arrow"/>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2362,7 +2621,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="106" name="Elbow Connector 105"/>
+        <xdr:cNvPr id="106" name="Elbow Connector 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="1"/>
           <a:endCxn id="8" idx="3"/>
@@ -2415,7 +2680,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="98" name="Elbow Connector 97"/>
+        <xdr:cNvPr id="98" name="Elbow Connector 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="22" idx="1"/>
           <a:endCxn id="8" idx="0"/>
@@ -2465,7 +2736,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="127" name="Flowchart: Connector 126"/>
+        <xdr:cNvPr id="127" name="Flowchart: Connector 126">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2514,25 +2791,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>303825</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>75225</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>351450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="130" name="Flowchart: Connector 129"/>
+        <xdr:cNvPr id="132" name="Flowchart: Connector 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000084000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4391025" y="2943225"/>
+          <a:off x="3829050" y="3429000"/>
           <a:ext cx="180000" cy="180000"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartConnector">
@@ -2576,68 +2859,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>56175</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="132" name="Flowchart: Connector 131"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3533775" y="3429000"/>
-          <a:ext cx="180000" cy="180000"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartConnector">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-        <a:ln w="3175">
-          <a:solidFill>
-            <a:srgbClr val="00B0F0"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>476251</xdr:colOff>
       <xdr:row>9</xdr:row>
@@ -2651,7 +2872,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="145" name="Rectangle 144"/>
+        <xdr:cNvPr id="145" name="Rectangle 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000091000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2725,7 +2952,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="146" name="Rectangle 145"/>
+        <xdr:cNvPr id="146" name="Rectangle 145">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000092000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2799,7 +3032,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="147" name="Rectangle 146"/>
+        <xdr:cNvPr id="147" name="Rectangle 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000093000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2869,11 +3108,555 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>475125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>182100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Fluxograma: Extrair 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D08F0D94-BC76-48F8-AE72-C295168DDB5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2303925" y="4991100"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>420225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>20175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Fluxograma: Extrair 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7761E3-8BE7-4C00-9BFA-CD958DBB4A2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1495425" y="5019675"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>191625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>29700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Fluxograma: Extrair 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D1971F-2A8C-4BF9-84E7-C77A110DE136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="657225" y="5029200"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>515475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4935</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Fluxograma: Extrair 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EADDCA7-5C82-4049-B014-9B181B7887B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4638675" y="2718435"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>134475</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>67800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Fluxograma: Extrair 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EF728F1-B66B-4FFC-8AB3-989D24186C0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9134475" y="5638800"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>96375</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>20175</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Fluxograma: Extrair 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62FAF86E-6B93-4292-8297-EA6624BD5E28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9096375" y="1781175"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>525000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Fluxograma: Extrair 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A46885D4-E871-4CA6-85B2-5C45058D9D9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1600200" y="971550"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>286875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Fluxograma: Extrair 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB54C84-80C3-41FC-B970-001BFF31FC57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2581275" y="971550"/>
+          <a:ext cx="144000" cy="144000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartExtract">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2915,7 +3698,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2948,9 +3731,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2983,6 +3783,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3159,16 +3976,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C5:R36"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L18" s="1"/>
+    </row>
+    <row r="31" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="36" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q36" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Bugs no gerenciamento das notificações Correção na conversõa de data e hora
</commit_message>
<xml_diff>
--- a/Documentos/Tasks.xlsx
+++ b/Documentos/Tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="9285"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -610,7 +610,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>AD</a:t>
+            <a:t>Data(AD)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3975,10 +3975,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:R36"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
@@ -4013,7 +4013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4025,7 +4025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>